<commit_message>
Fixed a regression bug & updated regex for search
- finder.py: Added an else statement which fixed the description being empty if the str was less than 2048 characters
  - Forgot to add the else statement in the last commit when "description" was introduced
- string_processing.py: Changed \b to \W at the end of the regex search pattern
  - Some strings werent being captured by \b, \W fixed that issue. Eg- née Wilkes!
- POS Dictionary json and xlsx were updated
</commit_message>
<xml_diff>
--- a/data/POS Dictionary.xlsx
+++ b/data/POS Dictionary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>Title</t>
   </si>
@@ -395,6 +395,142 @@
 • Ethics</t>
   </si>
   <si>
+    <t xml:space="preserve">LIST OF COMMON ABBREVIATIONS </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">• Soul Bond Curse (SBC) </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d curse`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Cryptohedron and Time-Turner (CATT) </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d time-turner`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Oath of Emnity (OoE) </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d ultimate`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Ultimate Sanction (US)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> (see `q.d ultimate`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Rune of Singular Hate (RoSH) </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d codex`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Wizengamot (WGT /  WZT) 
+• The Wizarding World (WW)
+• Word of God (WoG) </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see #pos-resources)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Molly's Magical Morsels (MMM / M3 / 3M)
+• Department of Mysteries (DoM) </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d early`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+• Ministry of Magic / Minister of Magic (MoM) 
+</t>
+    </r>
+  </si>
+  <si>
     <t>Advocatus Diaboli</t>
   </si>
   <si>
@@ -405,7 +541,8 @@
         <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">(First mentioned in Dreamscapes, Memories, and Nightmares (Pt. 1))
-(Requires a built Memory Palace) </t>
+(Requires a built Memory Palace) 
+</t>
     </r>
     <r>
       <rPr>
@@ -414,7 +551,7 @@
         <color rgb="FF000000"/>
         <sz val="12.0"/>
       </rPr>
-      <t>**Advocatus Diaboli:**</t>
+      <t>**Advocatus Diaboli**:</t>
     </r>
     <r>
       <rPr>
@@ -422,35 +559,108 @@
         <color rgb="FF000000"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve"> 
-A technique that allowed Snape to manifest a true secondary personality, one that was neither based on his own nor created from scratch. The Advocatus could give impartial advice and opinion on everything.</t>
+      <t xml:space="preserve"> A technique that allowed Snape to manifest a true secondary personality, one that was neither based on his own nor created from scratch. The Advocatus could give impartial advice and opinion on everything.</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">Perceptual Dilation / Time Dilation </t>
   </si>
   <si>
-    <t xml:space="preserve">(First mentioned in Home for the Holidays)
-(Needs at least 2nd level mastery) **Perceptual Dilation** or "*Fixing the Mind's Gaze Betwixt the Seven Beats of the Heart*": 
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(First mentioned in Home for the Holidays)
+(Needs at least 2nd level mastery) **</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Perceptual Dilation</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">** or "*Fixing the Mind's Gaze Betwixt the Seven Beats of the Heart*": 
 This technique slows down your subjective awareness of time, allowing you to study surroundings more thoroughly and make decisions more efficiently. Can only be maintained for a duration equal to seven beats of the Occlumen's heart. </t>
+    </r>
   </si>
   <si>
     <t>Tabula Rasa</t>
   </si>
   <si>
-    <t>(From The Fall of the House of Potter (pt 2))
-**Tabula Rasa**: A charm/curse invented to provide a humane alternative to the death penalty. 
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(From The Fall of the House of Potter (pt 2))
+**</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Tabula Rasa</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>**: A charm/curse invented to provide a humane alternative to the death penalty. 
 Totally erases the subject's memories and eliminates their ability to make new ones. Virtually lobotomizes the subject. 
-• Rookwood using incredibly advanced levels of occlumency has made him effectively immune to mind-alteration, emotional-manipulation, and memory-altering charms and potions of every kind. We also know that he is entirely immune to the Tabula Rasa. It is possible that he created at least 49 thought-streams while serving time in Azkaban. Using this 49-stream matrix he is able to generate and implant false personalities through some combination of wanded magic and Legilimency instead of his former tactic of implanting them slowly over the course of months through his cursed books. As long as Rookwood is free, the proliferation of sleeper-agents secretly loyal to Voldemort is a concern. 
-[See More](https://prince-of-slytherin.fandom.com/wiki/Augustus_Rookwood "Tip Toe Through the Tulips")</t>
+• Wizarding Australia uses it to "psychically execute" criminals convicted of capital crimes. They call it **Death of Personality**.
+• Rookwood using incredibly advanced levels of occlumency has made him effectively immune to mind-alteration, emotional-manipulation, and memory-altering charms and potions of every kind. We also know that he is entirely immune to the Tabula Rasa. 
+• It is possible that he created at least 49 thought-streams while serving time in Azkaban. Using this 49-stream matrix he is able to generate and implant false personalities through some combination of wanded magic and Legilimency instead of his former tactic of implanting them slowly over the course of months through his cursed books. 
+• As long as Rookwood is free, the proliferation of sleeper-agents secretly loyal to Voldemort is a concern. [See More](https://prince-of-slytherin.fandom.com/wiki/Augustus_Rookwood "Tip Toe Through the Tulips")</t>
+    </r>
   </si>
   <si>
     <t>Cryptohydron and Time-Turner (CATT)</t>
   </si>
   <si>
-    <t>(From The Hunting of Sirius Black (Conclusion) AN5)
-The **Cryptohedron** is a four-dimensional hypercube, and its changing shape is actually its three-dimensional shadow as it rotates, it houses the **Time-Turner** which is described as a glass tube that twists and turns back on itself, muggles would call it a Klein bottle. 
-• The Cryptohedron's purpose is to identify the one person who can open it and direct the Unspeakables to them at the appointed time so it can be opened and the Time Turner released. Both Time-Turner and container will be created at some point in the future and then sent back to the distant past. [See More](https://prince-of-slytherin.fandom.com/wiki/Time-Turner)</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(From The Hunting of Sirius Black (Conclusion) AN5)
+The **</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Cryptohedron</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>** is a four-dimensional hypercube, and its changing shape is actually its three-dimensional shadow as it rotates, it houses the **Time-Turner** which is described as a glass tube that twists and turns back on itself, muggles would call it a Klein bottle. 
+• The Cryptohedron's purpose is to identify the one person who can open it and direct the Unspeakables to them at the appointed time so it can be opened and the Time-Turner released. Both Time-Turner and container will be created at some point in the future and then sent back to the distant past. [See More](https://prince-of-slytherin.fandom.com/wiki/Time-Turner "Time is an illusion to help things make sense")</t>
+    </r>
   </si>
   <si>
     <t>Soul Bond Curse (SBC)</t>
@@ -528,7 +738,23 @@
         <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">(First mentioned in Happy Birthday, Harry and Jim!) 
-As a result of powerful and unnatural magics unleashed in 1927, the place known as </t>
+As a result of powerful and unnatural magics unleashed in 1927 </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d 7`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">, the place known as </t>
     </r>
     <r>
       <rPr>
@@ -589,16 +815,46 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t>** contains the 57 Chimes, which alert the Unspeakables to the events occuring in Magical Britain. According to Unspeakable 029, Broderick Bode, many of them were warnings of fairly innocuous events, and the most banal simply duplicated the warning systems of other departments as backups, whereas other chimes were less weird and more nightmarish. 
-[See More](https://prince-of-slytherin.fandom.com/wiki/Early_Warning_Office "More Like the DOOM Office")</t>
+      <t xml:space="preserve">**: contains the 57 Chimes, which alert the Unspeakables to the events occuring in Magical Britain. According to Unspeakable 029, Broderick Bode, many of them were warnings of fairly innocuous events, and the most banal simply duplicated the warning systems of other departments as backups, whereas other chimes were less weird and more nightmarish. [See More](https://prince-of-slytherin.fandom.com/wiki/Early_Warning_Office)
+Common Department Abbreviations: 
+• Department of Mysteries (DoM)
+• Ministry of Magic / Minister of Magic (MoM)
+• Department of Magical Law Enforcement (DMLE)
+• Department of Magical Games and Sports (DMGS)
+• Department Misuse of Muggle Artifacts  (MMA)
+</t>
     </r>
   </si>
   <si>
     <t>The Ewer of Hufflepuff</t>
   </si>
   <si>
-    <t>(From The Riddle of the Diary)
-the Ewer of Hufflepuff, created simultaneously with Slytherin's Basilisk will produce one full dose of the Restoration Potion every seventeen minutes.</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(From The Riddle of the Diary)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
+**The Ewer of Hufflepuff**</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>: created simultaneously with Slytherin's Basilisk will produce one full dose of the Restoration Potion every seventeen minutes.</t>
+    </r>
   </si>
   <si>
     <t>PoS Horcruxes / Horcrux</t>
@@ -705,18 +961,58 @@
     <t>Ley Lines</t>
   </si>
   <si>
-    <t>Invisible, intangible, and largely theoretical lines that criss-cross the whole planet. Can't actually be detected themselves, but the places where they connect are magically reactive. It is possible to do high level magic more easily than other locations and works spells whose results will last infinitely. 
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">**Ley Lines**: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Invisible, intangible, and largely theoretical lines that criss-cross the whole planet. Can't actually be detected themselves, but the places where they connect are magically reactive. It is possible to do high level magic more easily than other locations and works spells whose results will last infinitely. 
 • Hogwarts, the Ministry of Magic, Diagon Ally, and 12 Grimmauld Place are located at a junction of ley lines.
 • The British Isles possess an unusual number of such junctions and an extremely unusual number of junctions in which more than two ley lines intersect. That's why the original wizards came here from Rome in the first place. It's also why Magical Britain has influence over the rest of the magical world that's somewhat out of proportion to our population and the relative military and economic strength of the Muggle nation within which we reside. When push comes to shove, Britain can generate more raw magical power than all but a few of the other wizarding nations.</t>
+    </r>
   </si>
   <si>
     <t>Orichalcum</t>
   </si>
   <si>
-    <t xml:space="preserve">(First mentioned in The Birthday Part (Pt 1))
-An alchemically-produced alloy of gold and some other metal, usually copper or aluminum but sometimes silver or platinum. It's magic resistant, and if it's refined pure enough, it can slice through shield spells. 
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(First mentioned in The Birthday Part (Pt 1))
+**</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Orichalcum</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">**: An alchemically-produced alloy of gold and some other metal, usually copper or aluminum but sometimes silver or platinum. It's magic resistant, and if it's refined pure enough, it can slice through shield spells. 
 • Commercially available orichalcum is usually rated at about 50% pure. If you're willing to spend a fortune, orichalcum that is 65% pure can be obtained. About sixty years ago, Nicolas Flamel produced approximately twenty grams of orichalcum that was 75% pure, and he declared that further refinement beyond that point was absolutely impossible.
 • The box containing The Ring was made up of **&gt;85%** pure orichalcum. There is literally not enough galleons in Wizarding Britain to pay for such purity. Withstood fiendfyre without so much as a scratch. Can only be opened by Harry speaking parseltongue. </t>
+    </r>
   </si>
   <si>
     <t>FiendFyre</t>
@@ -747,7 +1043,7 @@
         <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">!'**
-In order to satisfy the esoteric requirement you must focus your mind on a memory of hating someone so much that you would die to ensure their destruction. So much, that you would see everyone left that you still cared about die along with you. 
+• In order to satisfy the esoteric requirement you must focus your mind on a memory of hating someone so much that you would die to ensure their destruction. So much, that you would see everyone left that you still cared about die along with you. 
 • Harry's and Regulus' fiendfyre flames take the shape of an enormous serpent and a wolf-like predator respectively. Described as daemonic antitheses of their patronuses. 
 • It is not considered a unforgivable because there are Class XXXXX creatures who can only be harmed by Fiendfyre. If you've summoned Fiendfyre and your opponent kills you, its flames will run wild, destroying your assailant as revenge. Along with everything within a few miles. 
 </t>
@@ -776,8 +1072,13 @@
     <t>Slytherin's Locket</t>
   </si>
   <si>
-    <t>• Originally kept in a cave from Tom's childhood, Regulus Black got Kreacher to help procure the locket and then charged his house-elf with destroying it while Regulus himself faked his own death and fled England. He was unable to retrieve the Locket until after freeing Sirius so that he could re-enter Grimmuald Place. Harry uses parseltongue to open the locket after first learning from the locket that Voldemort also used an object from Hufflepuff to make a Horcrux. The locket then takes the form of memories to torture both Harry and Regulus enough that they would be unable to destroy it. 
-• Harry destroys the Locket with a basilisk fang</t>
+    <t>(From Meet Regulus Black)
+The locket is described to be golden that bears a stylized "S" that usually appeared in depictions of Salazar Slytherin.
+• Originally kept in a cave set in a seaside cliff near Clacton-on-Sea, Voldemort uses Kreacher to test if the trap he has set to defend the locket works. The cave is surrounded by a lake that hides an army of inferi.  
+• Regulus Black commands Kreacher to lead him to the locket where Black drinks the foul potion designed to drive men mad. Then he charges his house-elf with destroying it. Due to the fatal thirst caused by the potion he is forced to drink from the inferi infested lake. He makes one last ditch effort to save himself and shapeshifts into Lord Voldemort (which scares the Inferi off) and manages to apparate away. 
+• Regulus discovers that the horcrux cannot be destroyed by elf magic and he does not have the esoteric requirements at the time to destroy it with fiendfyre. He then chooses to flee to Australia under the name of "Lazarus White". 
+• Harry uses parseltongue to open the locket after first learning from the S shaped snake on its front that Voldemort also used an object from Hufflepuff to make a Horcrux. The locket then takes the form of memories to torture both Harry and Regulus.
+• Harry eventually destroys the Locket with a basilisk fang</t>
   </si>
   <si>
     <t>The Diary / Thaumaturgical Organizing Matrix</t>
@@ -796,8 +1097,7 @@
     <t xml:space="preserve">Created by Helga Hufflepuff, she outlived the rest of the Founders by three decades. 
 • Destroyed by Harry after he asked the group who wanted to keep it and who wanted to destroy it. Everyone in the room who had strong Occlumency defenses wanted to destroy the horcrux immedietly, while everyone who *didn't* was making excuses for keeping it around indefinitely until they could figure out how to *use* it. 
 • Bellatrix informed Harry that the Cup in currently in her vault at Gringotts and only she is able to recover it due to bio-magical signature security placed on the vault that she ensured was on the vault when her master entrusted her with a valuable item. One of these measures include the use of the  Flagrante-Gemino Curse.
-• At its base has the words *Vinum Bibistus* inscribed which translates to *"Drink Wine"*. Lucius identifies the inscription from *Rubaiyat* a collection of 11th century poetry written by Omar Khayyam. The full passage goes: "*Drink wine. This life is eternal. This is all that youth will give you. It is the season for wine, roses, and drunken friends. Be happy for this moment. This moment is your life*". 
-</t>
+• At its base has the words *Vinum Bibistus* inscribed which translates to *"Drink Wine"*. Lucius identifies the inscription from *Rubaiyat* a collection of 11th century poetry written by Omar Khayyam. The full [passage](https://libquotes.com/omar-khayy%C3%A1m/quote/lbt4u8r "this is a real thing") goes: "*Drink wine. This life is eternal. This is all that youth will give you. It is the season for wine, roses, and drunken friends. Be happy for this moment. This moment is your life*". </t>
   </si>
   <si>
     <t>Imago Dei</t>
@@ -842,9 +1142,9 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve"> that can literally re-write reality to the casters wishes. It's literal translation in English is 'Image of God'. 
+      <t xml:space="preserve"> that can literally re-write reality to the caster's wishes. Its literal translation in English is 'Image of God'. 
 • Imago Dei is the first spell from the Anathema Codex seen being performed "on-screen".
-• The second is The Rune of Singular Hate was used during the attack on Hogsmeade. 
+• The second is The Rune of Singular Hate which was used during the attack on Hogsmeade. 
 [See More](https://prince-of-slytherin.fandom.com/wiki/Imago_Dei "Image of God")</t>
     </r>
   </si>
@@ -874,7 +1174,7 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t>), which have been deemed too dangerous to society should they become public knowledge. It contains spells, rituals, potions, procedures for breeding unnatural beasts, and ancient runes. 
+      <t xml:space="preserve">), which have been deemed too dangerous to society should they become public knowledge. It contains spells, rituals, potions, procedures for breeding unnatural beasts, and ancient runes. 
 __List of spells which are known to be contained within:__
   •  The Lament Configuration
   •  The Bane of Sicily
@@ -884,7 +1184,23 @@
   •  The Feast of Shadows
   •  The Inverted Mirror
   •  The Hounds of Tindalos
-  •  Imago Dei
+  •  Imago Dei </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF4285F4"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>(see `q.d 17`)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">
   •  The Horcrux Ritual
 [See More](https://prince-of-slytherin.fandom.com/wiki/Anathema_Codex "Not to be confused with Anne #6204")</t>
     </r>
@@ -894,8 +1210,7 @@
   </si>
   <si>
     <t>The **Azkaban Conspiracy**, also known as the **Azkabal**, was the group responsible for the July 31, 1993 Azkaban breakout. The group was initiated by Regulus Black, who had been planning this for years. 
-• The group's primary objective was to free Sirius Black, Rophuldus Lestrange, Rastaban Lestrange, Bellatrix Lestrange, and Augustus Rookwood from Azkaban's high security track. Sirius was freed because he is innocent and Regulus brother, the other four were taken for their potential knowledge of Lord Voldemort's Horcruxes. 
-[See More](https://prince-of-slytherin.fandom.com/wiki/Azkaban_Conspiracy ")</t>
+• The group's primary objective was to free Sirius Black, Rophuldus Lestrange, Rastaban Lestrange, Bellatrix Lestrange, and Augustus Rookwood from Azkaban's high security track. Sirius was freed because he is innocent and Regulus brother, the other four were taken for their potential knowledge of Lord Voldemort's Horcruxes. [See More](https://prince-of-slytherin.fandom.com/wiki/Azkaban_Conspiracy)</t>
   </si>
   <si>
     <t>Wild Magic</t>
@@ -903,8 +1218,7 @@
   <si>
     <t>**Wild Magic** is Magic in its raw form, can be summed up in eight simple words: `'As I will it, so mote it be.'` Wizards have spent millennia striving to limit magic's potential, to ensure that magic is irrevocably linked to wands and incantations, defined as charms and transfigurations and potions, and restrained by the principles of arithmancy and runic matrices. The minute a compatible wand is picked up at Olivander's, those sparks that shot out represent the one's promise as a wizard that they would work magic according to the principles taught at magical schools, like Hogwarts. 
 • *Accidental Magic is the simplest form of Wild Magic.* 
-• It is theorized that **Wild Magic** is what is keeping Harry's scar from being identified as a Sowilō rune along with messing with a lot of other things in Harry's life. 
-[See More](https://prince-of-slytherin.fandom.com/wiki/Wild_Magic "Where the Wild Things Are")</t>
+• It is theorized that **Wild Magic** is what is keeping Harry's scar from being identified as a Sowilō rune along with messing with a lot of other things in Harry's life. [See More](https://prince-of-slytherin.fandom.com/wiki/Wild_Magic "Wheels Within Wheels")</t>
   </si>
   <si>
     <t xml:space="preserve">Memory Palace </t>
@@ -915,7 +1229,20 @@
 • Once properly developed can store your most sensitive memories in a partitioned area of your mind and can protect them with psychic traps capable of harming those who push too far. 
 • A Memory palace can be used to store false personalities that can be draped over your true self
 • False memory palaces can be created as Legilimancy traps to harm those who walk in. Jim gets trapped within Diary Riddle's memory palace 
-• Vasyl Dobroshtan (from Beauxbatons) created a technique for embedding psychic attacks inside artwork designed to magically draw and hold the viewer's undivided attention. One of his creations was a *Cruciatus Curse* conveyed through art. Rufus Scrimgeour locked this image away in his Memory Palace and uses it to fight back against Rookwood during The Fall of the House of Potter (Pt 1).</t>
+• Vasyl Dobroshtan (from Beauxbatons) created a technique for embedding psychic attacks inside artwork designed to magically draw and hold the viewer's undivided attention. One of his creations was a *Cruciatus Curse* conveyed through art. Rufus Scrimgeour locked this image away in his Memory Palace and uses it to fight back against Rookwood during *The Fall of the House of Potter (Pt 1)*.</t>
+  </si>
+  <si>
+    <t>Ultimate Sanction (US)</t>
+  </si>
+  <si>
+    <t>**The Ultimate Sanction**, also known as *Sanctumen Ultimo*, is a provision of the Inheritance Act of 1588 that gives any Wizengamot House's Head the ability to disown a member of their House if the Head judges that the member has committed treason against their House or has committed actions that, if left unchallenged, threatens the survival of that House. 
+When activated, the recipient will be forcefully removed from their House, with the recipient's surname becoming "No-Name", and losing any ties to their former house, including inheritance. [See More](https://prince-of-slytherin.fandom.com/wiki/The_Ultimate_Sanction)</t>
+  </si>
+  <si>
+    <t>WoG / WZT / WGT / 3M / MoM / OoE</t>
+  </si>
+  <si>
+    <t>see (`q.d abbreviations`)</t>
   </si>
 </sst>
 </file>
@@ -982,11 +1309,11 @@
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
@@ -1013,19 +1340,19 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1288,7 +1615,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2"/>
@@ -1317,10 +1644,10 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" ht="43.5" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
@@ -1352,7 +1679,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2"/>
@@ -1384,7 +1711,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2"/>
@@ -1669,8 +1996,12 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -29328,185 +29659,193 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="42.75" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>26</v>
+      <c r="A2" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" ht="42.75" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" ht="102.75" customHeight="1">
-      <c r="A4" s="15" t="s">
+    <row r="3" ht="42.75" customHeight="1">
+      <c r="A3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="4" ht="102.75" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="5" ht="42.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>33</v>
+      <c r="B5" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" ht="42.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="42.75" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" ht="42.75" customHeight="1">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>1927.0</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>38</v>
+      <c r="B8" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" ht="42.75" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" ht="42.75" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" ht="42.75" customHeight="1">
-      <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B10" s="13" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="11" ht="42.75" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="12" ht="42.75" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>46</v>
+      <c r="B12" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" ht="42.75" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>48</v>
+      <c r="B13" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" ht="42.75" customHeight="1">
-      <c r="A15" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" ht="42.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+    <row r="15" ht="42.75" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" ht="42.75" customHeight="1">
-      <c r="A17" s="11" t="s">
+    <row r="16" ht="42.75" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" ht="42.75" customHeight="1">
-      <c r="A18" s="11" t="s">
+    <row r="17" ht="42.75" customHeight="1">
+      <c r="A17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B17" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" ht="42.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+    <row r="18" ht="42.75" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B18" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" ht="42.75" customHeight="1">
-      <c r="A20" s="11" t="s">
+    <row r="19" ht="42.75" customHeight="1">
+      <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" ht="42.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+    <row r="20" ht="42.75" customHeight="1">
+      <c r="A20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>64</v>
       </c>
     </row>
+    <row r="21" ht="42.75" customHeight="1">
+      <c r="A21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="22" ht="42.75" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>66</v>
+      <c r="B22" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" ht="42.75" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="24" ht="42.75" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" ht="42.75" customHeight="1">
       <c r="A25" s="12"/>

</xml_diff>